<commit_message>
Excel export added in angular
</commit_message>
<xml_diff>
--- a/LearnAPI/wwwroot/Export/customerinfo.xlsx
+++ b/LearnAPI/wwwroot/Export/customerinfo.xlsx
@@ -34,37 +34,85 @@
     <x:t>1</x:t>
   </x:si>
   <x:si>
-    <x:t>sanjeev</x:t>
-  </x:si>
-  <x:si>
-    <x:t>sanjeev@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>7598798722</x:t>
+    <x:t>sanjeev praj</x:t>
+  </x:si>
+  <x:si>
+    <x:t>prajapatisanjiv8@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8799879871</x:t>
   </x:si>
   <x:si>
     <x:t>2</x:t>
   </x:si>
   <x:si>
-    <x:t>bala</x:t>
-  </x:si>
-  <x:si>
-    <x:t>bala@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>198739811</x:t>
+    <x:t>balasaheb</x:t>
+  </x:si>
+  <x:si>
+    <x:t>balasaheb.more@cloverinfotech.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7368768761</x:t>
   </x:si>
   <x:si>
     <x:t>3</x:t>
   </x:si>
   <x:si>
-    <x:t>viraj damani</x:t>
+    <x:t>viraj</x:t>
   </x:si>
   <x:si>
     <x:t>viraj@gmail.com</x:t>
   </x:si>
   <x:si>
-    <x:t>789182981</x:t>
+    <x:t>8768768761</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>rajesh</x:t>
+  </x:si>
+  <x:si>
+    <x:t>rajesh@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>83987987987</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>bipin tiwariii</x:t>
+  </x:si>
+  <x:si>
+    <x:t>bipin@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>82739879898</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>saideep</x:t>
+  </x:si>
+  <x:si>
+    <x:t>saideep@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21837987981</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>test</x:t>
+  </x:si>
+  <x:si>
+    <x:t>test@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3009739711</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -128,8 +176,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E4" totalsRowShown="0">
-  <x:autoFilter ref="A1:E4"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E8" totalsRowShown="0">
+  <x:autoFilter ref="A1:E8"/>
   <x:tableColumns count="5">
     <x:tableColumn id="1" name="Code"/>
     <x:tableColumn id="2" name="Name"/>
@@ -429,7 +477,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E4"/>
+  <x:dimension ref="A1:E8"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -466,7 +514,7 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="E2" s="0">
-        <x:v>100000</x:v>
+        <x:v>100090</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5">
@@ -483,7 +531,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="E3" s="0">
-        <x:v>20000</x:v>
+        <x:v>9999</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:5">
@@ -500,7 +548,75 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="E4" s="0">
-        <x:v>400000</x:v>
+        <x:v>190000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:5">
+      <x:c r="A5" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E5" s="0">
+        <x:v>10000000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:5">
+      <x:c r="A6" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="E6" s="0">
+        <x:v>9999999</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:5">
+      <x:c r="A7" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="E7" s="0">
+        <x:v>440000</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:5">
+      <x:c r="A8" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="E8" s="0">
+        <x:v>19991</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>